<commit_message>
add function:makeclass save excel log
</commit_message>
<xml_diff>
--- a/ClassData/24Class.xlsx
+++ b/ClassData/24Class.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonProject\AttributeProgram\ClassData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23250" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="ClassData" sheetId="2" r:id="rId1"/>
@@ -22,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="295">
   <si>
     <t>idx</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2131,7 +2126,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2166,7 +2161,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2377,7 +2372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2787,10 +2782,10 @@
         <v>2</v>
       </c>
       <c r="G14" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="33">
         <v>3</v>
@@ -3309,10 +3304,10 @@
         <v>3</v>
       </c>
       <c r="G32" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" s="33">
         <v>5</v>
@@ -3625,7 +3620,7 @@
         <v>84</v>
       </c>
       <c r="F43" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G43" s="34">
         <v>0</v>
@@ -3683,13 +3678,13 @@
         <v>86</v>
       </c>
       <c r="F45" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G45" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" s="33">
         <v>7</v>
@@ -3828,7 +3823,7 @@
         <v>180</v>
       </c>
       <c r="F50" s="37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G50" s="34">
         <v>0</v>
@@ -3857,7 +3852,7 @@
         <v>180</v>
       </c>
       <c r="F51" s="37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G51" s="34">
         <v>0</v>
@@ -3886,7 +3881,7 @@
         <v>180</v>
       </c>
       <c r="F52" s="37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G52" s="34">
         <v>0</v>
@@ -3915,7 +3910,7 @@
         <v>180</v>
       </c>
       <c r="F53" s="37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G53" s="34">
         <v>0</v>
@@ -3944,7 +3939,7 @@
         <v>180</v>
       </c>
       <c r="F54" s="37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G54" s="34">
         <v>0</v>
@@ -3973,7 +3968,7 @@
         <v>180</v>
       </c>
       <c r="F55" s="37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G55" s="34">
         <v>0</v>
@@ -4118,7 +4113,7 @@
         <v>160</v>
       </c>
       <c r="F60" s="37">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G60" s="34">
         <v>0</v>
@@ -4147,7 +4142,7 @@
         <v>173</v>
       </c>
       <c r="F61" s="37">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G61" s="34">
         <v>0</v>
@@ -4176,7 +4171,7 @@
         <v>161</v>
       </c>
       <c r="F62" s="37">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G62" s="34">
         <v>0</v>
@@ -4205,7 +4200,7 @@
         <v>174</v>
       </c>
       <c r="F63" s="37">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G63" s="34">
         <v>0</v>
@@ -4263,7 +4258,7 @@
         <v>181</v>
       </c>
       <c r="F65" s="37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G65" s="34">
         <v>0</v>
@@ -4292,7 +4287,7 @@
         <v>181</v>
       </c>
       <c r="F66" s="37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G66" s="34">
         <v>0</v>
@@ -4321,7 +4316,7 @@
         <v>181</v>
       </c>
       <c r="F67" s="37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G67" s="34">
         <v>0</v>
@@ -4379,7 +4374,7 @@
         <v>181</v>
       </c>
       <c r="F69" s="37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G69" s="34">
         <v>0</v>
@@ -4408,7 +4403,7 @@
         <v>181</v>
       </c>
       <c r="F70" s="37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G70" s="34">
         <v>0</v>
@@ -4495,7 +4490,7 @@
         <v>181</v>
       </c>
       <c r="F73" s="37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G73" s="34">
         <v>0</v>
@@ -4835,11 +4830,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4897,10 +4890,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="63">
-        <v>14</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>278</v>
+        <v>10</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -4908,10 +4901,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="63">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>59</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -4919,20 +4912,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="63">
+        <v>18</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="67">
+        <v>7</v>
+      </c>
+      <c r="B8" s="63">
         <v>19</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C8" s="57" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5">
+    <row r="9" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="69">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
         <v>20</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C9" s="59" t="s">
         <v>284</v>
       </c>
     </row>
@@ -4947,7 +4951,7 @@
   <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>